<commit_message>
atualização de padreão de funções e comentários
</commit_message>
<xml_diff>
--- a/R/microssimulation/data/dic_variables.xlsx
+++ b/R/microssimulation/data/dic_variables.xlsx
@@ -3521,8 +3521,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009FCF1CFFB8E2FD48B98C1D289E6F7434" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="993932be92d286f244708a7079812cf8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60b9ac05-b026-4e06-8db0-0531ef559a77" xmlns:ns3="fdf6d43d-45dd-43b3-a524-6e9101d49666" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="592646d8aaa64f8b8eb2cb91b3f10e7e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009FCF1CFFB8E2FD48B98C1D289E6F7434" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="144d7f9580aa2fc5017ab48860158dfa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60b9ac05-b026-4e06-8db0-0531ef559a77" xmlns:ns3="fdf6d43d-45dd-43b3-a524-6e9101d49666" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f9e074bd034d5d46739eb6d4f322db1" ns2:_="" ns3:_="">
     <xsd:import namespace="60b9ac05-b026-4e06-8db0-0531ef559a77"/>
     <xsd:import namespace="fdf6d43d-45dd-43b3-a524-6e9101d49666"/>
     <xsd:element name="properties">
@@ -3546,6 +3546,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3621,6 +3622,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fdf6d43d-45dd-43b3-a524-6e9101d49666" elementFormDefault="qualified">
@@ -3773,7 +3779,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E5CB29-3FB8-4764-AFDD-CA7F99228C8D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ED4FB64-04CF-4F3A-9F61-D68E68BE6457}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>